<commit_message>
process run coding completed but data layer.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/inventory_operation_record_test_cases.xlsx
+++ b/soberano/test_cases/inventory_operation_record_test_cases.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="material_expense_record_test_ca" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="inventory operation record test" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -430,13 +430,13 @@
   </sheetPr>
   <dimension ref="A1:AMJ48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="W19" activeCellId="0" sqref="W19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.12"/>
@@ -455,7 +455,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="22.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="14.35"/>

</xml_diff>